<commit_message>
add product detail,product and catogory manager screen
</commit_message>
<xml_diff>
--- a/Home/data/master_data.xlsx
+++ b/Home/data/master_data.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Da mặt" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Body" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Trang điểm" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Tóc mi mày" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Nước hoa" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="Viên uống bổ sung" sheetId="6" r:id="rId8"/>
+    <sheet name="Da mặt" sheetId="1" r:id="rId1"/>
+    <sheet name="Body" sheetId="2" r:id="rId2"/>
+    <sheet name="Trang điểm" sheetId="3" r:id="rId3"/>
+    <sheet name="Tóc mi mày" sheetId="4" r:id="rId4"/>
+    <sheet name="Nước hoa" sheetId="5" r:id="rId5"/>
+    <sheet name="Viên uống bổ sung" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -622,149 +626,565 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="7">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0"/>
+    <cellStyle name="Percent" xfId="15"/>
+    <cellStyle name="Currency" xfId="16"/>
+    <cellStyle name="Currency [0]" xfId="17"/>
+    <cellStyle name="Comma" xfId="18"/>
+    <cellStyle name="Comma [0]" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -772,22 +1192,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.86"/>
-    <col customWidth="1" min="2" max="2" width="12.43"/>
-    <col customWidth="1" min="3" max="3" width="47.14"/>
-    <col customWidth="1" min="4" max="4" width="53.0"/>
-    <col customWidth="1" min="7" max="7" width="43.29"/>
-    <col customWidth="1" min="9" max="9" width="53.86"/>
-    <col customWidth="1" min="10" max="10" width="105.86"/>
-    <col customWidth="1" min="12" max="12" width="23.14"/>
+    <col min="1" max="1" width="5.85714285714286" customWidth="1"/>
+    <col min="2" max="2" width="12.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="47.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="7" max="7" width="43.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="53.8571428571429" customWidth="1"/>
+    <col min="10" max="10" width="105.857142857143" customWidth="1"/>
+    <col min="12" max="12" width="23.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,12 +1234,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -827,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="7">
-        <v>1350000.0</v>
+        <v>1350000</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>30</v>
@@ -839,12 +1260,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>46</v>
@@ -853,7 +1274,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="7">
-        <v>1158000.0</v>
+        <v>1158000</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>51</v>
@@ -862,12 +1283,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>58</v>
@@ -876,7 +1297,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="7">
-        <v>1022000.0</v>
+        <v>1022000</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>63</v>
@@ -885,12 +1306,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>69</v>
@@ -899,7 +1320,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="7">
-        <v>3700000.0</v>
+        <v>3700000</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>63</v>
@@ -908,12 +1329,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>78</v>
@@ -922,7 +1343,7 @@
         <v>81</v>
       </c>
       <c r="E6" s="7">
-        <v>1242000.0</v>
+        <v>1242000</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>51</v>
@@ -931,12 +1352,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>86</v>
@@ -945,7 +1366,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="7">
-        <v>4427000.0</v>
+        <v>4427000</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>14</v>
@@ -954,12 +1375,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>91</v>
@@ -968,7 +1389,7 @@
         <v>93</v>
       </c>
       <c r="E8" s="7">
-        <v>682000.0</v>
+        <v>682000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>95</v>
@@ -981,12 +1402,12 @@
       </c>
       <c r="M8" s="10"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>99</v>
@@ -995,7 +1416,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="7">
-        <v>5000000.0</v>
+        <v>5000000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>14</v>
@@ -1010,12 +1431,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" ht="15.75">
       <c r="A10" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>104</v>
@@ -1024,7 +1445,7 @@
         <v>105</v>
       </c>
       <c r="E10" s="3">
-        <v>3225000.0</v>
+        <v>3225000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>30</v>
@@ -1035,12 +1456,12 @@
       <c r="L10" s="13"/>
       <c r="M10" s="14"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" ht="15.75">
       <c r="A11" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>107</v>
@@ -1049,7 +1470,7 @@
         <v>108</v>
       </c>
       <c r="E11" s="3">
-        <v>1910000.0</v>
+        <v>1910000</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>21</v>
@@ -1060,7 +1481,7 @@
       <c r="L11" s="15"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12">
+    <row r="12" spans="2:8" ht="15.75">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1069,7 +1490,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="2:8" ht="15.75">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1078,7 +1499,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:8" ht="15.75">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1087,7 +1508,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:8" ht="15.75">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1096,35 +1517,35 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16">
+    <row r="16" spans="4:8" ht="15.75">
       <c r="D16" s="5"/>
       <c r="E16" s="7"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="4:8" ht="15.75">
       <c r="D17" s="5"/>
       <c r="E17" s="7"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="4:8" ht="15.75">
       <c r="D18" s="5"/>
       <c r="E18" s="7"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19">
+    <row r="19" spans="4:8" ht="15.75">
       <c r="D19" s="5"/>
       <c r="E19" s="7"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="2:8" ht="15.75">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1133,7 +1554,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="2:8" ht="15.75">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1142,110 +1563,111 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22">
+    <row r="22" spans="5:6" ht="15.75">
       <c r="E22" s="17"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23">
+    <row r="23" spans="5:6" ht="15.75">
       <c r="E23" s="17"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24">
+    <row r="24" spans="5:6" ht="15.75">
       <c r="E24" s="17"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25">
+    <row r="25" spans="5:6" ht="15.75">
       <c r="E25" s="17"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26">
+    <row r="26" spans="5:6" ht="15.75">
       <c r="E26" s="17"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27">
+    <row r="27" spans="5:6" ht="15.75">
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28">
+    <row r="28" ht="15.75">
       <c r="F28" s="18"/>
     </row>
-    <row r="29">
+    <row r="29" ht="15.75">
       <c r="F29" s="18"/>
     </row>
-    <row r="30">
+    <row r="30" ht="15.75">
       <c r="F30" s="18"/>
     </row>
-    <row r="31">
+    <row r="31" ht="15.75">
       <c r="F31" s="18"/>
     </row>
-    <row r="32">
+    <row r="32" ht="15.75">
       <c r="F32" s="18"/>
     </row>
-    <row r="33">
+    <row r="33" ht="15.75">
       <c r="F33" s="18"/>
     </row>
-    <row r="34">
+    <row r="34" ht="15.75">
       <c r="F34" s="18"/>
     </row>
-    <row r="35">
+    <row r="35" ht="15.75">
       <c r="F35" s="18"/>
     </row>
-    <row r="36">
+    <row r="36" ht="15.75">
       <c r="F36" s="18"/>
     </row>
-    <row r="37">
+    <row r="37" ht="15.75">
       <c r="F37" s="18"/>
     </row>
-    <row r="38">
+    <row r="38" ht="15.75">
       <c r="F38" s="18"/>
     </row>
-    <row r="39">
+    <row r="39" ht="15.75">
       <c r="F39" s="18"/>
     </row>
-    <row r="40">
+    <row r="40" ht="15.75">
       <c r="F40" s="18"/>
     </row>
-    <row r="41">
+    <row r="41" ht="15.75">
       <c r="F41" s="18"/>
     </row>
-    <row r="42">
+    <row r="42" ht="15.75">
       <c r="F42" s="18"/>
     </row>
-    <row r="43">
+    <row r="43" ht="15.75">
       <c r="F43" s="18"/>
     </row>
-    <row r="44">
+    <row r="44" ht="15.75">
       <c r="F44" s="18"/>
     </row>
-    <row r="45">
+    <row r="45" ht="15.75">
       <c r="F45" s="18"/>
     </row>
-    <row r="46">
+    <row r="46" ht="15.75">
       <c r="F46" s="18"/>
     </row>
-    <row r="47">
+    <row r="47" ht="15.75">
       <c r="F47" s="18"/>
     </row>
-    <row r="48">
+    <row r="48" ht="15.75">
       <c r="F48" s="18"/>
     </row>
-    <row r="49">
+    <row r="49" ht="15.75">
       <c r="F49" s="18"/>
     </row>
-    <row r="50">
+    <row r="50" ht="15.75">
       <c r="F50" s="18"/>
     </row>
-    <row r="51">
+    <row r="51" ht="15.75">
       <c r="F51" s="18"/>
     </row>
-    <row r="52">
+    <row r="52" ht="15.75">
       <c r="F52" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="M9:M11"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1254,17 +1676,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="40.29"/>
-    <col customWidth="1" min="4" max="4" width="59.29"/>
-    <col customWidth="1" min="7" max="7" width="35.86"/>
+    <col min="3" max="3" width="40.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="59.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="35.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1293,12 +1716,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -1307,7 +1730,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="3">
-        <v>2157000.0</v>
+        <v>2157000</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1319,12 +1742,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>19</v>
@@ -1333,7 +1756,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="3">
-        <v>790000.0</v>
+        <v>790000</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>21</v>
@@ -1342,12 +1765,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>25</v>
@@ -1356,7 +1779,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="3">
-        <v>450000.0</v>
+        <v>450000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>21</v>
@@ -1365,12 +1788,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>33</v>
@@ -1379,7 +1802,7 @@
         <v>34</v>
       </c>
       <c r="E5" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -1388,12 +1811,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
@@ -1402,7 +1825,7 @@
         <v>40</v>
       </c>
       <c r="E6" s="3">
-        <v>849000.0</v>
+        <v>849000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>30</v>
@@ -1411,12 +1834,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>47</v>
@@ -1425,7 +1848,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="3">
-        <v>950000.0</v>
+        <v>950000</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>14</v>
@@ -1434,12 +1857,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>57</v>
@@ -1448,7 +1871,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="3">
-        <v>2015000.0</v>
+        <v>2015000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>62</v>
@@ -1457,12 +1880,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>68</v>
@@ -1471,7 +1894,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="3">
-        <v>2112000.0</v>
+        <v>2112000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>63</v>
@@ -1480,12 +1903,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>77</v>
@@ -1494,7 +1917,7 @@
         <v>80</v>
       </c>
       <c r="E10" s="3">
-        <v>1800000.0</v>
+        <v>1800000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>30</v>
@@ -1503,8 +1926,10 @@
         <v>83</v>
       </c>
     </row>
+    <row r="11" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1513,18 +1938,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="45.0"/>
-    <col customWidth="1" min="4" max="4" width="58.71"/>
-    <col customWidth="1" min="7" max="7" width="62.0"/>
-    <col customWidth="1" min="8" max="8" width="19.71"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="4" width="58.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="62" customWidth="1"/>
+    <col min="8" max="8" width="19.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1550,12 +1976,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -1564,7 +1990,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="3">
-        <v>1600000.0</v>
+        <v>1600000</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1576,12 +2002,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
@@ -1590,7 +2016,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="3">
-        <v>950000.0</v>
+        <v>950000</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>26</v>
@@ -1599,12 +2025,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>31</v>
@@ -1613,7 +2039,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="3">
-        <v>649000.0</v>
+        <v>649000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>21</v>
@@ -1622,12 +2048,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>37</v>
@@ -1636,7 +2062,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="3">
-        <v>1000000.0</v>
+        <v>1000000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -1645,12 +2071,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>45</v>
@@ -1659,7 +2085,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="3">
-        <v>1250000.0</v>
+        <v>1250000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -1668,12 +2094,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>55</v>
@@ -1682,7 +2108,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="3">
-        <v>550000.0</v>
+        <v>550000</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>14</v>
@@ -1691,12 +2117,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>66</v>
@@ -1705,7 +2131,7 @@
         <v>67</v>
       </c>
       <c r="E8" s="3">
-        <v>520000.0</v>
+        <v>520000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>14</v>
@@ -1714,12 +2140,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>75</v>
@@ -1728,7 +2154,7 @@
         <v>76</v>
       </c>
       <c r="E9" s="3">
-        <v>810000.0</v>
+        <v>810000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>21</v>
@@ -1737,12 +2163,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>84</v>
@@ -1751,7 +2177,7 @@
         <v>85</v>
       </c>
       <c r="E10" s="3">
-        <v>360000.0</v>
+        <v>360000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>26</v>
@@ -1760,12 +2186,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>90</v>
@@ -1774,7 +2200,7 @@
         <v>92</v>
       </c>
       <c r="E11" s="3">
-        <v>2150000.0</v>
+        <v>2150000</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>94</v>
@@ -1783,8 +2209,10 @@
         <v>97</v>
       </c>
     </row>
+    <row r="12" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1793,17 +2221,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="61.86"/>
-    <col customWidth="1" min="4" max="4" width="49.71"/>
-    <col customWidth="1" min="7" max="7" width="39.14"/>
+    <col min="3" max="3" width="61.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="49.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="39.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1829,12 +2258,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>114</v>
@@ -1843,7 +2272,7 @@
         <v>116</v>
       </c>
       <c r="E2" s="3">
-        <v>1500000.0</v>
+        <v>1500000</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -1855,12 +2284,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>123</v>
@@ -1869,7 +2298,7 @@
         <v>125</v>
       </c>
       <c r="E3" s="3">
-        <v>2800000.0</v>
+        <v>2800000</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
@@ -1878,12 +2307,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>133</v>
@@ -1892,7 +2321,7 @@
         <v>134</v>
       </c>
       <c r="E4" s="3">
-        <v>1100000.0</v>
+        <v>1100000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>14</v>
@@ -1901,12 +2330,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>140</v>
@@ -1915,7 +2344,7 @@
         <v>142</v>
       </c>
       <c r="E5" s="3">
-        <v>1122000.0</v>
+        <v>1122000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -1924,12 +2353,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>148</v>
@@ -1938,7 +2367,7 @@
         <v>149</v>
       </c>
       <c r="E6" s="3">
-        <v>515000.0</v>
+        <v>515000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>14</v>
@@ -1947,12 +2376,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>156</v>
@@ -1961,7 +2390,7 @@
         <v>158</v>
       </c>
       <c r="E7" s="3">
-        <v>2149000.0</v>
+        <v>2149000</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>14</v>
@@ -1970,12 +2399,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>160</v>
@@ -1984,7 +2413,7 @@
         <v>161</v>
       </c>
       <c r="E8" s="3">
-        <v>1750000.0</v>
+        <v>1750000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>14</v>
@@ -1993,12 +2422,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>163</v>
@@ -2007,7 +2436,7 @@
         <v>164</v>
       </c>
       <c r="E9" s="3">
-        <v>3203000.0</v>
+        <v>3203000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>14</v>
@@ -2016,12 +2445,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>166</v>
@@ -2030,7 +2459,7 @@
         <v>167</v>
       </c>
       <c r="E10" s="3">
-        <v>795000.0</v>
+        <v>795000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>14</v>
@@ -2039,8 +2468,10 @@
         <v>168</v>
       </c>
     </row>
+    <row r="11" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2049,17 +2480,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="34.14"/>
-    <col customWidth="1" min="4" max="4" width="48.14"/>
-    <col customWidth="1" min="7" max="7" width="48.29"/>
+    <col min="3" max="3" width="34.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="48.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="48.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2085,12 +2517,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>110</v>
@@ -2099,7 +2531,7 @@
         <v>111</v>
       </c>
       <c r="E2" s="3">
-        <v>1395000.0</v>
+        <v>1395000</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>30</v>
@@ -2111,12 +2543,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>115</v>
@@ -2125,7 +2557,7 @@
         <v>117</v>
       </c>
       <c r="E3" s="3">
-        <v>9300000.0</v>
+        <v>9300000</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>30</v>
@@ -2134,12 +2566,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>121</v>
@@ -2148,7 +2580,7 @@
         <v>122</v>
       </c>
       <c r="E4" s="3">
-        <v>2780000.0</v>
+        <v>2780000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>30</v>
@@ -2157,12 +2589,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>126</v>
@@ -2171,7 +2603,7 @@
         <v>127</v>
       </c>
       <c r="E5" s="3">
-        <v>8500000.0</v>
+        <v>8500000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>30</v>
@@ -2180,12 +2612,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>130</v>
@@ -2194,7 +2626,7 @@
         <v>131</v>
       </c>
       <c r="E6" s="3">
-        <v>4005000.0</v>
+        <v>4005000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>30</v>
@@ -2203,12 +2635,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>135</v>
@@ -2217,7 +2649,7 @@
         <v>136</v>
       </c>
       <c r="E7" s="3">
-        <v>3770000.0</v>
+        <v>3770000</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>30</v>
@@ -2226,12 +2658,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>139</v>
@@ -2240,7 +2672,7 @@
         <v>141</v>
       </c>
       <c r="E8" s="3">
-        <v>5160000.0</v>
+        <v>5160000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>30</v>
@@ -2249,12 +2681,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>145</v>
@@ -2263,7 +2695,7 @@
         <v>146</v>
       </c>
       <c r="E9" s="3">
-        <v>3141000.0</v>
+        <v>3141000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>14</v>
@@ -2272,12 +2704,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>150</v>
@@ -2286,7 +2718,7 @@
         <v>151</v>
       </c>
       <c r="E10" s="3">
-        <v>1521000.0</v>
+        <v>1521000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>14</v>
@@ -2295,12 +2727,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>154</v>
@@ -2309,7 +2741,7 @@
         <v>155</v>
       </c>
       <c r="E11" s="3">
-        <v>2370000.0</v>
+        <v>2370000</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>14</v>
@@ -2318,8 +2750,10 @@
         <v>157</v>
       </c>
     </row>
+    <row r="12" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2328,17 +2762,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="49.29"/>
-    <col customWidth="1" min="4" max="4" width="64.71"/>
-    <col customWidth="1" min="7" max="7" width="54.57"/>
+    <col min="3" max="3" width="49.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="64.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="54.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2364,12 +2799,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>169</v>
@@ -2378,7 +2813,7 @@
         <v>170</v>
       </c>
       <c r="E2" s="3">
-        <v>3800000.0</v>
+        <v>3800000</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -2390,12 +2825,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>173</v>
@@ -2404,7 +2839,7 @@
         <v>174</v>
       </c>
       <c r="E3" s="3">
-        <v>900000.0</v>
+        <v>900000</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
@@ -2413,12 +2848,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>176</v>
@@ -2427,7 +2862,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="3">
-        <v>1282600.0</v>
+        <v>1282600</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>178</v>
@@ -2436,12 +2871,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>180</v>
@@ -2450,7 +2885,7 @@
         <v>181</v>
       </c>
       <c r="E5" s="3">
-        <v>2600180.0</v>
+        <v>2600180</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>178</v>
@@ -2459,12 +2894,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>183</v>
@@ -2473,7 +2908,7 @@
         <v>184</v>
       </c>
       <c r="E6" s="3">
-        <v>2465000.0</v>
+        <v>2465000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -2482,12 +2917,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>186</v>
@@ -2496,7 +2931,7 @@
         <v>187</v>
       </c>
       <c r="E7" s="3">
-        <v>1704000.0</v>
+        <v>1704000</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>14</v>
@@ -2505,12 +2940,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>189</v>
@@ -2519,7 +2954,7 @@
         <v>190</v>
       </c>
       <c r="E8" s="3">
-        <v>1350000.0</v>
+        <v>1350000</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>21</v>
@@ -2528,12 +2963,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>192</v>
@@ -2542,7 +2977,7 @@
         <v>193</v>
       </c>
       <c r="E9" s="3">
-        <v>1575000.0</v>
+        <v>1575000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>21</v>
@@ -2551,12 +2986,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>195</v>
@@ -2565,7 +3000,7 @@
         <v>196</v>
       </c>
       <c r="E10" s="3">
-        <v>1200000.0</v>
+        <v>1200000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>21</v>
@@ -2574,7 +3009,9 @@
         <v>197</v>
       </c>
     </row>
+    <row r="11" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish product detail 80% - error: cannot binding image
</commit_message>
<xml_diff>
--- a/Home/data/master_data.xlsx
+++ b/Home/data/master_data.xlsx
@@ -2221,7 +2221,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -2284,7 +2284,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2480,7 +2480,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -2543,7 +2543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75">
+    <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="3">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix 1 dong bug
</commit_message>
<xml_diff>
--- a/Home/data/master_data.xlsx
+++ b/Home/data/master_data.xlsx
@@ -2768,7 +2768,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -2831,7 +2831,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75">
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add entity framework + update 1 dong cho :v
</commit_message>
<xml_diff>
--- a/Home/data/master_data.xlsx
+++ b/Home/data/master_data.xlsx
@@ -1265,7 +1265,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="5">
         <v>0</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75">
+    <row r="12" spans="2:8" ht="12.75">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75">
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -1944,7 +1944,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -2008,7 +2008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75">
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75">
+    <row r="11" spans="1:7" ht="12.75">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2227,7 +2227,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -2290,7 +2290,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75">
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="3">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add category status, icon when add new category, edit category
</commit_message>
<xml_diff>
--- a/Home/data/master_data.xlsx
+++ b/Home/data/master_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="200">
   <si>
     <t>Status</t>
   </si>
@@ -607,6 +607,21 @@
   </si>
   <si>
     <t>Nước uống làm sáng da Astalift White Drink Whiteshield giúp làm sáng da, giúp ngăn ngừa oxi hóa và kiểm soát tác hại của tia UV đối với làn da, mang đến làn da trắng sáng khỏe mạnh.</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Sữa tắm từ bò</t>
+  </si>
+  <si>
+    <t>default.jpg</t>
+  </si>
+  <si>
+    <t>Trung Quốc</t>
+  </si>
+  <si>
+    <t>đồ trung quốc đừng có dùng</t>
   </si>
 </sst>
 </file>
@@ -3025,7 +3040,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -3057,6 +3072,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:9" ht="12.75">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2">
+        <v>2000000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9"/>

</xml_diff>